<commit_message>
Updated to use utc time stamp
git-tfs-id: [https://payerportfolio.visualstudio.com/]$/USHC_AMER_US_ADU_HSP_Ua3/Source/Utilities/Dev;C1598384
</commit_message>
<xml_diff>
--- a/components/Oracle to SQL Comparison.xlsx
+++ b/components/Oracle to SQL Comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xmabdulkhayum\Desktop\Mediaiddailycall\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UA3\Source\Utilities\Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FC3C05-F486-445E-9EBE-7B5A4562D80C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2480B46B-7201-4D88-9E04-027D13080F41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="600" windowWidth="18400" windowHeight="10200" firstSheet="1" activeTab="1" xr2:uid="{6185548A-CE3F-4A8C-BB72-B234B9DAD96E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{6185548A-CE3F-4A8C-BB72-B234B9DAD96E}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL to Oracle Syntax" sheetId="1" state="hidden" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="215">
   <si>
     <t>Change Databases in SQL Server vs. Oracle</t>
   </si>
@@ -586,9 +586,6 @@
     <t>Index Creation in SQL Server vs. Oracle</t>
   </si>
   <si>
-    <t>WITH (DATA_COMPRESSION = NONE)</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO </t>
   </si>
   <si>
@@ -600,9 +597,6 @@
   </si>
   <si>
     <t>Add FK Constraint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	EXEC sp_rename N'UA3_TPL_POLICY.POTENTIAL_TPL_CLAIM_PK', N'PAID_CLAIM_PK', N'OBJECT'</t>
   </si>
   <si>
     <t>alter table PAID_CLAIM 
@@ -618,9 +612,6 @@
     <t>Rename FK Constraint</t>
   </si>
   <si>
-    <t>EXEC sp_rename N'UA3_TPL_POLICY.POTENTIAL_TPL_CLAIM_FK0', N'PAID_CLAIM_FK0', N'OBJECT'</t>
-  </si>
-  <si>
     <t>Mention Data Compression</t>
   </si>
   <si>
@@ -628,14 +619,7 @@
   on PROVIDER_LICENSE(LICENSE_NUMBER_TXT); </t>
   </si>
   <si>
-    <t>CREATE INDEX [PROVIDER_LICENSE_IX0] 
-  ON [UA3_SCREENING].[PROVIDER_LICENSE]</t>
-  </si>
-  <si>
     <t>(LICENSE_NUMBER_TXT)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  WITH (SORT_IN_TEMPDB = OFF, DROP_EXISTING = OFF, IGNORE_DUP_KEY = OFF, ONLINE = ON) ON [PRIMARY]; </t>
   </si>
   <si>
     <t>ALTER TABLE TENANT 
@@ -647,16 +631,6 @@
   <si>
     <t>ALTER TABLE TENANT
 ADD TENANT_NAME varchar(150) NULL;</t>
-  </si>
-  <si>
-    <t>ALTER TABLE [UA3_TENANT].[TENANT] 
-ALTER COLUMN TENANT_NAME varchar(200) NOT NULL
-GO</t>
-  </si>
-  <si>
-    <t>ALTER TABLE [UA3_TENANT].[TENANT]
-ADD [TENANT_NAME] varchar(150) NULL
-GO</t>
   </si>
   <si>
     <t>EXEC SP_RENAME 'UA3_TPL_POLICY.POTENTIAL_TPL_CLAIM', 'PAID_CLAIM'
@@ -700,13 +674,156 @@
 AND EVENT_TYPENAME = 'HIPPExpenditureRequestUpdated';</t>
   </si>
   <si>
+    <t>Adding transaction scope for multiple (Insert/Update/Delete) DML statements.</t>
+  </si>
+  <si>
+    <t>begin tran
+		update [UA3_INTEGRATION].[MODULE_EVENTS] set [EVENT_TYPE_NAME] = 'ExpenditureRequestApproved', [MODIFIED_TS] = GETDATE()
+		where [EVENT_TYPE_NAME] = 'HIPPExpenditureRequestApproved';
+	commit;
+GO</t>
+  </si>
+  <si>
+    <t>update UA3_INTEGRATION.MODULE_EVENTS set EVENT_TYPE_NAME = 'ExpenditureRequestApproved', MODIFIED_TS = SYSDATE
+where EVENT_TYPE_NAME = 'HIPPExpenditureRequestApproved';
+commit;</t>
+  </si>
+  <si>
+    <t>Blob to clob/
+Clob to blob (function) and how to use in queries</t>
+  </si>
+  <si>
+    <t>Adding transaction scope for single (Insert/Update/Delete) DML statement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exec sp_help  [UA3_INTEGRATION].[MODULE_EVENTS]
+</t>
+  </si>
+  <si>
+    <t>describe UA3_INTEGRATION.MODULE_EVENTS</t>
+  </si>
+  <si>
+    <t>To read a table definition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Table Creation</t>
+  </si>
+  <si>
+    <t>Index Creation</t>
+  </si>
+  <si>
+    <t>Add column to a existing table.</t>
+  </si>
+  <si>
+    <t>Modify a column datatype with NULL\NOT NULL constraint in a existing table.</t>
+  </si>
+  <si>
+    <t>Modify a column datatype in a existing table.</t>
+  </si>
+  <si>
+    <t>Rename a Primary key.</t>
+  </si>
+  <si>
+    <t>Create a Foreign key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a Primary key </t>
+  </si>
+  <si>
+    <t>Rename a Foreign key</t>
+  </si>
+  <si>
+    <t>create table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [APP_ID] uniqueidentifier  not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [APP_NAME] varchar(100)  not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [IS_ACTIVE] bit  not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [LAST_MODIFIED_TS] datetime2(6)  not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [MODULE_ID] uniqueidentifier  null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [APP_TYPE] varchar(10)  null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [APP_DESC] varchar(1000)  null</t>
+  </si>
+  <si>
+    <t>with (data_compression = none)</t>
+  </si>
+  <si>
+    <t>create index [PROVIDER_LICENSE_IX0] 
+  on [UA3_SCREENING].[PROVIDER_LICENSE]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  with (sort_in_tempdb = off, drop_existing = off, ignore_dup_key = off, online = on) on [primary]; </t>
+  </si>
+  <si>
+    <t>alter table [UA3_TENANT].[TENANT]
+add [TENANT_NAME] varchar(150) null
+GO</t>
+  </si>
+  <si>
+    <t>alter table [UA3_TENANT].[APPLICATION]</t>
+  </si>
+  <si>
+    <t>alter table [UA3_TENANT].[TENANT] 
+alter column TENANT_NAME varchar(200) not null
+GO</t>
+  </si>
+  <si>
+    <t>exec sp_rename 
+'UA3_INTEGRATION.ETF_OUTBOUND_METADATA_DEFN.ETF_OUTBOUND_EXTRACT_ID', 
+'ETF_OUTBOUND_EXTRACT_NAME', 'COLUMN' 
+GO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	exec sp_rename  N'UA3_TPL_POLICY.POTENTIAL_TPL_CLAIM_PK', N'PAID_CLAIM_PK', N'OBJECT'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    on delete no action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    on update no action</t>
+  </si>
+  <si>
+    <t>exec sp_rename N'UA3_TPL_POLICY.POTENTIAL_TPL_CLAIM_FK0', N'PAID_CLAIM_FK0', N'OBJECT'</t>
+  </si>
+  <si>
+    <t>INSERT INTO APPLICATION
+    (
+      APP_ID,	    APP_NAME,	    IS_ACTIVE,    LAST_MODIFIED_TS	  )
+	  VALUES
+	  (
+      newid(),	    'Auth Determination Services',	    1,	    getutcdate()	  );</t>
+  </si>
+  <si>
+    <t>SELECT SYS_GUID() 
+INTO V_QUERY_SERVICE_APP_ID
+  FROM DUAL;	  
+INSERT INTO APPLICATION
+(
+APP_ID, APP_NAME,IS_ACTIVE,LAST_MODIFIED_TS)
+VALUES
+(
+V_QUERY_SERVICE_APP_ID,'Auth Determination Services',	1,sys_extract_utc(systimestamp));</t>
+  </si>
+  <si>
     <t>begin try
 	begin tran
-		update [UA3_INTEGRATION].[MODULE_EVENTS] set [EVENT_TYPE_NAME] = 'ExpenditureRequestApproved', [MODIFIED_TS] = GETDATE()
+		update [UA3_INTEGRATION].[MODULE_EVENTS] set [EVENT_TYPE_NAME] = 'ExpenditureRequestApproved', [MODIFIED_TS] = getutcdate()
 		where [EVENT_TYPE_NAME] = 'HIPPExpenditureRequestApproved';
-		update [UA3_INTEGRATION].[MODULE_EVENTS] set [EVENT_TYPE_NAME] = 'ExpenditureRequestRejected', [MODIFIED_TS] = GETDATE() 
+		update [UA3_INTEGRATION].[MODULE_EVENTS] set [EVENT_TYPE_NAME] = 'ExpenditureRequestRejected', [MODIFIED_TS] = getutcdate() 
 		where [EVENT_TYPE_NAME] = 'HIPPExpenditureRequestRejected';
-		update [UA3_INTEGRATION].[MODULE_EVENTS] set [EVENT_TYPE_NAME] = 'ExpenditureRequestUpdated', [MODIFIED_TS] = GETDATE() 
+		update [UA3_INTEGRATION].[MODULE_EVENTS] set [EVENT_TYPE_NAME] = 'ExpenditureRequestUpdated', [MODIFIED_TS] = getutcdate() 
 		where [EVENT_TYPE_NAME] = 'HIPPExpenditureRequestUpdated';
 	commit;
 end try
@@ -723,72 +840,13 @@
 GO</t>
   </si>
   <si>
-    <t>update UA3_INTEGRATION.MODULE_EVENTS set EVENT_TYPE_NAME = 'ExpenditureRequestApproved', MODIFIED_TS = SYSDATE
+    <t>update UA3_INTEGRATION.MODULE_EVENTS set EVENT_TYPE_NAME = 'ExpenditureRequestApproved', MODIFIED_TS = sys_extract_utc(systimestamp)
 where EVENT_TYPE_NAME = 'HIPPExpenditureRequestApproved';
-update UA3_INTEGRATION.MODULE_EVENTS set EVENT_TYPE_NAME = 'ExpenditureRequestRejected', MODIFIED_TS = SYSDATE 
+update UA3_INTEGRATION.MODULE_EVENTS set EVENT_TYPE_NAME = 'ExpenditureRequestRejected', MODIFIED_TS = sys_extract_utc(systimestamp)
 where EVENT_TYPE_NAME = 'HIPPExpenditureRequestRejected';
-update UA3_INTEGRATION.MODULE_EVENTS set EVENT_TYPE_NAME = 'ExpenditureRequestUpdated', MODIFIED_TS = SYSDATE 
+update UA3_INTEGRATION.MODULE_EVENTS set EVENT_TYPE_NAME = 'ExpenditureRequestUpdated', MODIFIED_TS = sys_extract_utc(systimestamp) 
 where EVENT_TYPE_NAME = 'HIPPExpenditureRequestUpdated'; 
 commit;</t>
-  </si>
-  <si>
-    <t>Adding transaction scope for multiple (Insert/Update/Delete) DML statements.</t>
-  </si>
-  <si>
-    <t>begin tran
-		update [UA3_INTEGRATION].[MODULE_EVENTS] set [EVENT_TYPE_NAME] = 'ExpenditureRequestApproved', [MODIFIED_TS] = GETDATE()
-		where [EVENT_TYPE_NAME] = 'HIPPExpenditureRequestApproved';
-	commit;
-GO</t>
-  </si>
-  <si>
-    <t>update UA3_INTEGRATION.MODULE_EVENTS set EVENT_TYPE_NAME = 'ExpenditureRequestApproved', MODIFIED_TS = SYSDATE
-where EVENT_TYPE_NAME = 'HIPPExpenditureRequestApproved';
-commit;</t>
-  </si>
-  <si>
-    <t>Blob to clob/
-Clob to blob (function) and how to use in queries</t>
-  </si>
-  <si>
-    <t>Adding transaction scope for single (Insert/Update/Delete) DML statement.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exec sp_help  [UA3_INTEGRATION].[MODULE_EVENTS]
-</t>
-  </si>
-  <si>
-    <t>describe UA3_INTEGRATION.MODULE_EVENTS</t>
-  </si>
-  <si>
-    <t>To read a table definition.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Table Creation</t>
-  </si>
-  <si>
-    <t>Index Creation</t>
-  </si>
-  <si>
-    <t>Add column to a existing table.</t>
-  </si>
-  <si>
-    <t>Modify a column datatype with NULL\NOT NULL constraint in a existing table.</t>
-  </si>
-  <si>
-    <t>Modify a column datatype in a existing table.</t>
-  </si>
-  <si>
-    <t>Rename a Primary key.</t>
-  </si>
-  <si>
-    <t>Create a Foreign key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create a Primary key </t>
-  </si>
-  <si>
-    <t>Rename a Foreign key</t>
   </si>
 </sst>
 </file>
@@ -1513,13 +1571,13 @@
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="52.26953125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="52.28515625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="51.26953125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="60.81640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="44.26953125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="29.7265625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="52.26953125" style="8"/>
+    <col min="1" max="1" width="51.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="60.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="52.28515625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1544,7 +1602,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="46.5">
+    <row r="3" spans="1:4" ht="47.25">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -1556,7 +1614,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="31">
+    <row r="4" spans="1:4" ht="31.5">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -1584,7 +1642,7 @@
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
     </row>
-    <row r="7" spans="1:4" ht="108.5">
+    <row r="7" spans="1:4" ht="105.75">
       <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
@@ -1686,7 +1744,7 @@
       <c r="C16" s="28"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="30.75">
       <c r="A17" s="11" t="s">
         <v>19</v>
       </c>
@@ -1748,7 +1806,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="31">
+    <row r="23" spans="1:5" ht="30.75">
       <c r="A23" s="11" t="s">
         <v>26</v>
       </c>
@@ -1774,7 +1832,7 @@
       <c r="C25" s="31"/>
       <c r="D25" s="35"/>
     </row>
-    <row r="26" spans="1:5" ht="46.5" hidden="1">
+    <row r="26" spans="1:5" ht="47.25" hidden="1">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1805,7 +1863,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="77.5">
+    <row r="28" spans="1:5" ht="78.75">
       <c r="A28" s="1" t="s">
         <v>113</v>
       </c>
@@ -1995,7 +2053,7 @@
       <c r="C46" s="28"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" ht="31">
+    <row r="47" spans="1:4" ht="31.5">
       <c r="A47" s="15" t="s">
         <v>137</v>
       </c>
@@ -2071,7 +2129,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="62">
+    <row r="55" spans="1:4" ht="63">
       <c r="A55" s="16" t="s">
         <v>47</v>
       </c>
@@ -2081,7 +2139,7 @@
       <c r="C55" s="28"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" ht="31.5">
       <c r="A56" s="5" t="s">
         <v>48</v>
       </c>
@@ -2099,7 +2157,7 @@
       <c r="C57" s="31"/>
       <c r="D57" s="35"/>
     </row>
-    <row r="58" spans="1:4" ht="46.5">
+    <row r="58" spans="1:4" ht="45.75">
       <c r="A58" s="11" t="s">
         <v>49</v>
       </c>
@@ -2139,7 +2197,7 @@
       <c r="C61" s="31"/>
       <c r="D61" s="35"/>
     </row>
-    <row r="62" spans="1:4" ht="46.5">
+    <row r="62" spans="1:4" ht="45.75">
       <c r="A62" s="11" t="s">
         <v>53</v>
       </c>
@@ -2149,7 +2207,7 @@
       <c r="C62" s="28"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4" ht="46.5">
+    <row r="63" spans="1:4" ht="45.75">
       <c r="B63" s="11" t="s">
         <v>121</v>
       </c>
@@ -2249,7 +2307,7 @@
       <c r="C73" s="32"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4" ht="46.5">
+    <row r="74" spans="1:4" ht="47.25">
       <c r="A74" s="19" t="s">
         <v>70</v>
       </c>
@@ -2325,7 +2383,7 @@
       <c r="C82" s="32"/>
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="1:4" ht="31">
+    <row r="83" spans="1:4" ht="31.5">
       <c r="A83" s="21" t="s">
         <v>78</v>
       </c>
@@ -2343,7 +2401,7 @@
       <c r="C84" s="33"/>
       <c r="D84" s="35"/>
     </row>
-    <row r="85" spans="1:4" ht="31">
+    <row r="85" spans="1:4" ht="30.75">
       <c r="A85" s="18" t="s">
         <v>79</v>
       </c>
@@ -2369,7 +2427,7 @@
       <c r="C87" s="32"/>
       <c r="D87" s="3"/>
     </row>
-    <row r="88" spans="1:4" ht="31">
+    <row r="88" spans="1:4" ht="31.5">
       <c r="A88" s="19" t="s">
         <v>82</v>
       </c>
@@ -2431,7 +2489,7 @@
       <c r="C94" s="32"/>
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:4" ht="31">
+    <row r="95" spans="1:4" ht="31.5">
       <c r="A95" s="21" t="s">
         <v>88</v>
       </c>
@@ -2505,7 +2563,7 @@
       <c r="C102" s="32"/>
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="1:4" ht="31">
+    <row r="103" spans="1:4" ht="31.5">
       <c r="A103" s="21" t="s">
         <v>95</v>
       </c>
@@ -2567,7 +2625,7 @@
       <c r="C109" s="33"/>
       <c r="D109" s="35"/>
     </row>
-    <row r="110" spans="1:4" ht="31">
+    <row r="110" spans="1:4" ht="30.75">
       <c r="A110" s="18" t="s">
         <v>99</v>
       </c>
@@ -2648,25 +2706,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31552E27-7043-4734-AF5E-4A430D897916}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69:D70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="49.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="49.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.81640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5">
+    <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="28"/>
     </row>
-    <row r="2" spans="1:4" ht="15.5">
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -2678,19 +2736,19 @@
       </c>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" ht="15.5">
+    <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="11" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="49" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.5">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
@@ -2702,7 +2760,7 @@
       </c>
       <c r="D4" s="50"/>
     </row>
-    <row r="5" spans="1:4" ht="15.5">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
@@ -2712,9 +2770,9 @@
       <c r="C5" s="28"/>
       <c r="D5" s="50"/>
     </row>
-    <row r="6" spans="1:4" ht="15.5">
+    <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="11" t="s">
-        <v>16</v>
+        <v>193</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>128</v>
@@ -2722,9 +2780,9 @@
       <c r="C6" s="28"/>
       <c r="D6" s="50"/>
     </row>
-    <row r="7" spans="1:4" ht="15.5">
+    <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="11" t="s">
-        <v>17</v>
+        <v>194</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>129</v>
@@ -2732,9 +2790,9 @@
       <c r="C7" s="28"/>
       <c r="D7" s="50"/>
     </row>
-    <row r="8" spans="1:4" ht="15.5">
+    <row r="8" spans="1:4" ht="15.75">
       <c r="A8" s="11" t="s">
-        <v>18</v>
+        <v>195</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>130</v>
@@ -2742,9 +2800,9 @@
       <c r="C8" s="28"/>
       <c r="D8" s="50"/>
     </row>
-    <row r="9" spans="1:4" ht="31">
+    <row r="9" spans="1:4" ht="30.75">
       <c r="A9" s="11" t="s">
-        <v>19</v>
+        <v>196</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>131</v>
@@ -2752,9 +2810,9 @@
       <c r="C9" s="28"/>
       <c r="D9" s="50"/>
     </row>
-    <row r="10" spans="1:4" ht="15.5">
+    <row r="10" spans="1:4" ht="15.75">
       <c r="A10" s="11" t="s">
-        <v>20</v>
+        <v>197</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>132</v>
@@ -2762,9 +2820,9 @@
       <c r="C10" s="28"/>
       <c r="D10" s="50"/>
     </row>
-    <row r="11" spans="1:4" ht="15.5">
+    <row r="11" spans="1:4" ht="15.75">
       <c r="A11" s="11" t="s">
-        <v>21</v>
+        <v>198</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>133</v>
@@ -2772,9 +2830,9 @@
       <c r="C11" s="28"/>
       <c r="D11" s="50"/>
     </row>
-    <row r="12" spans="1:4" ht="15.5">
+    <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="11" t="s">
-        <v>22</v>
+        <v>199</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>134</v>
@@ -2782,7 +2840,7 @@
       <c r="C12" s="28"/>
       <c r="D12" s="50"/>
     </row>
-    <row r="13" spans="1:4" ht="15.5">
+    <row r="13" spans="1:4" ht="15.75">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -2792,17 +2850,17 @@
       <c r="C13" s="28"/>
       <c r="D13" s="50"/>
     </row>
-    <row r="14" spans="1:4" ht="15.5">
+    <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="1" t="s">
-        <v>151</v>
+        <v>200</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="28" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D14" s="50"/>
     </row>
-    <row r="15" spans="1:4" ht="15.5">
+    <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
@@ -2812,7 +2870,7 @@
       </c>
       <c r="D15" s="50"/>
     </row>
-    <row r="16" spans="1:4" ht="31">
+    <row r="16" spans="1:4" ht="30.75">
       <c r="A16" s="11" t="s">
         <v>26</v>
       </c>
@@ -2820,7 +2878,7 @@
       <c r="C16" s="28"/>
       <c r="D16" s="50"/>
     </row>
-    <row r="17" spans="1:4" ht="15.5">
+    <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="5" t="s">
         <v>150</v>
       </c>
@@ -2828,7 +2886,7 @@
       <c r="C17" s="28"/>
       <c r="D17" s="51"/>
     </row>
-    <row r="18" spans="1:4" ht="15.5">
+    <row r="18" spans="1:4" ht="15.75">
       <c r="A18" s="9" t="s">
         <v>1</v>
       </c>
@@ -2838,19 +2896,19 @@
       <c r="C18" s="31"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" ht="46.5">
+    <row r="19" spans="1:4" ht="45.75">
       <c r="A19" s="11" t="s">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="52" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.5">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
@@ -2858,15 +2916,15 @@
       <c r="C20" s="28"/>
       <c r="D20" s="53"/>
     </row>
-    <row r="21" spans="1:4" ht="15.5">
+    <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="28"/>
       <c r="D21" s="53"/>
     </row>
-    <row r="22" spans="1:4" ht="15.5">
+    <row r="22" spans="1:4" ht="15.75">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
@@ -2874,23 +2932,23 @@
       <c r="C22" s="28"/>
       <c r="D22" s="53"/>
     </row>
-    <row r="23" spans="1:4" ht="46.5">
+    <row r="23" spans="1:4" ht="45.75">
       <c r="A23" s="11" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="28"/>
       <c r="D23" s="53"/>
     </row>
-    <row r="24" spans="1:4" ht="15.5">
+    <row r="24" spans="1:4" ht="15.75">
       <c r="A24" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="28"/>
       <c r="D24" s="53"/>
     </row>
-    <row r="25" spans="1:4" ht="15.5">
+    <row r="25" spans="1:4" ht="15.75">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -2898,7 +2956,7 @@
       <c r="C25" s="28"/>
       <c r="D25" s="54"/>
     </row>
-    <row r="26" spans="1:4" ht="15.5">
+    <row r="26" spans="1:4" ht="15.75">
       <c r="A26" s="9" t="s">
         <v>1</v>
       </c>
@@ -2908,65 +2966,65 @@
       <c r="C26" s="31"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" ht="46.5">
+    <row r="27" spans="1:4" ht="47.25">
       <c r="A27" s="38" t="s">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="62">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="63">
       <c r="A28" s="3" t="s">
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="62">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="63">
       <c r="A29" s="3" t="s">
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="B29" s="37" t="s">
         <v>112</v>
       </c>
       <c r="C29" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="41" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="62">
+    </row>
+    <row r="30" spans="1:4" ht="63">
       <c r="A30" s="3" t="s">
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="77.5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="78.75">
       <c r="A31" s="39" t="s">
-        <v>146</v>
+        <v>206</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>144</v>
@@ -2975,24 +3033,24 @@
         <v>145</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="62">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="63">
       <c r="A32" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C32" s="28" t="s">
         <v>147</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.5">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75">
       <c r="A33" s="5" t="s">
         <v>35</v>
       </c>
@@ -3000,7 +3058,7 @@
       <c r="C33" s="28"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" ht="15.5">
+    <row r="34" spans="1:4" ht="15.75">
       <c r="A34" s="9" t="s">
         <v>1</v>
       </c>
@@ -3010,21 +3068,21 @@
       <c r="C34" s="31"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:4" ht="15.5">
+    <row r="35" spans="1:4" ht="30.75">
       <c r="A35" s="11" t="s">
-        <v>36</v>
+        <v>204</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75">
       <c r="A36" s="11" t="s">
         <v>38</v>
       </c>
@@ -3034,7 +3092,7 @@
       <c r="C36" s="28"/>
       <c r="D36" s="53"/>
     </row>
-    <row r="37" spans="1:4" ht="15.5">
+    <row r="37" spans="1:4" ht="15.75">
       <c r="A37" s="11" t="s">
         <v>39</v>
       </c>
@@ -3044,7 +3102,7 @@
       <c r="C37" s="28"/>
       <c r="D37" s="53"/>
     </row>
-    <row r="38" spans="1:4" ht="15.5">
+    <row r="38" spans="1:4" ht="15.75">
       <c r="A38" s="11" t="s">
         <v>41</v>
       </c>
@@ -3052,7 +3110,7 @@
       <c r="C38" s="28"/>
       <c r="D38" s="53"/>
     </row>
-    <row r="39" spans="1:4" ht="15.5">
+    <row r="39" spans="1:4" ht="15.75">
       <c r="A39" s="15" t="s">
         <v>6</v>
       </c>
@@ -3060,21 +3118,21 @@
       <c r="C39" s="28"/>
       <c r="D39" s="54"/>
     </row>
-    <row r="40" spans="1:4" ht="46.5">
+    <row r="40" spans="1:4" ht="47.25">
       <c r="A40" s="15" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>149</v>
       </c>
       <c r="D40" s="55" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75">
       <c r="A41" s="15" t="s">
         <v>6</v>
       </c>
@@ -3082,13 +3140,13 @@
       <c r="C41" s="28"/>
       <c r="D41" s="56"/>
     </row>
-    <row r="42" spans="1:4" ht="15.5">
+    <row r="42" spans="1:4" ht="15.75">
       <c r="A42" s="15"/>
       <c r="B42" s="11"/>
       <c r="C42" s="28"/>
       <c r="D42" s="56"/>
     </row>
-    <row r="43" spans="1:4" ht="15.5">
+    <row r="43" spans="1:4" ht="15.75">
       <c r="A43" s="5" t="s">
         <v>42</v>
       </c>
@@ -3096,7 +3154,7 @@
       <c r="C43" s="28"/>
       <c r="D43" s="57"/>
     </row>
-    <row r="44" spans="1:4" ht="15.5">
+    <row r="44" spans="1:4" ht="15.75">
       <c r="A44" s="9" t="s">
         <v>1</v>
       </c>
@@ -3106,21 +3164,21 @@
       <c r="C44" s="31"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:4" ht="15.5">
+    <row r="45" spans="1:4" ht="30.75">
       <c r="A45" s="11" t="s">
-        <v>36</v>
+        <v>204</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D45" s="55" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75">
       <c r="A46" s="11" t="s">
         <v>136</v>
       </c>
@@ -3130,7 +3188,7 @@
       <c r="C46" s="28"/>
       <c r="D46" s="56"/>
     </row>
-    <row r="47" spans="1:4" ht="15.5">
+    <row r="47" spans="1:4" ht="15.75">
       <c r="A47" s="11" t="s">
         <v>139</v>
       </c>
@@ -3140,7 +3198,7 @@
       <c r="C47" s="28"/>
       <c r="D47" s="56"/>
     </row>
-    <row r="48" spans="1:4" ht="15.5">
+    <row r="48" spans="1:4" ht="15.75">
       <c r="A48" s="11" t="s">
         <v>108</v>
       </c>
@@ -3150,7 +3208,7 @@
       <c r="C48" s="28"/>
       <c r="D48" s="56"/>
     </row>
-    <row r="49" spans="1:4" ht="31">
+    <row r="49" spans="1:4" ht="31.5">
       <c r="A49" s="15" t="s">
         <v>137</v>
       </c>
@@ -3158,44 +3216,44 @@
       <c r="C49" s="28"/>
       <c r="D49" s="56"/>
     </row>
-    <row r="50" spans="1:4" ht="15.5">
+    <row r="50" spans="1:4" ht="15.75">
       <c r="A50" s="15" t="s">
-        <v>43</v>
+        <v>208</v>
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="28"/>
       <c r="D50" s="56"/>
     </row>
-    <row r="51" spans="1:4" ht="15.5">
+    <row r="51" spans="1:4" ht="15.75">
       <c r="A51" s="15" t="s">
-        <v>44</v>
+        <v>209</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="28"/>
       <c r="D51" s="56"/>
     </row>
-    <row r="52" spans="1:4" ht="15.5">
+    <row r="52" spans="1:4" ht="15.75">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D52" s="57"/>
     </row>
-    <row r="53" spans="1:4" ht="62">
+    <row r="53" spans="1:4" ht="60.75">
       <c r="A53" s="1" t="s">
-        <v>160</v>
+        <v>210</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C53" s="28"/>
       <c r="D53" s="42" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.5">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75">
       <c r="A54" s="1" t="s">
         <v>6</v>
       </c>
@@ -3203,13 +3261,13 @@
       <c r="C54" s="28"/>
       <c r="D54" s="11"/>
     </row>
-    <row r="55" spans="1:4" ht="15.5">
+    <row r="55" spans="1:4" ht="15.75">
       <c r="A55" s="1"/>
       <c r="B55" s="11"/>
       <c r="C55" s="28"/>
       <c r="D55" s="11"/>
     </row>
-    <row r="56" spans="1:4" ht="15.5">
+    <row r="56" spans="1:4" ht="31.5">
       <c r="A56" s="5" t="s">
         <v>45</v>
       </c>
@@ -3217,7 +3275,7 @@
       <c r="C56" s="28"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="1:4" ht="15.5">
+    <row r="57" spans="1:4" ht="15.75">
       <c r="A57" s="9" t="s">
         <v>1</v>
       </c>
@@ -3227,19 +3285,19 @@
       <c r="C57" s="31"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="1:4" ht="170.5">
+    <row r="58" spans="1:4" ht="180.75">
       <c r="A58" s="11" t="s">
-        <v>115</v>
+        <v>211</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>119</v>
+        <v>212</v>
       </c>
       <c r="C58" s="28"/>
       <c r="D58" s="43" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15.5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75">
       <c r="A59" s="11" t="s">
         <v>46</v>
       </c>
@@ -3247,7 +3305,7 @@
       <c r="C59" s="28"/>
       <c r="D59" s="11"/>
     </row>
-    <row r="60" spans="1:4" ht="62">
+    <row r="60" spans="1:4" ht="63">
       <c r="A60" s="16" t="s">
         <v>47</v>
       </c>
@@ -3256,10 +3314,10 @@
       </c>
       <c r="C60" s="28"/>
       <c r="D60" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="31">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="31.5">
       <c r="A61" s="5" t="s">
         <v>48</v>
       </c>
@@ -3267,7 +3325,7 @@
       <c r="C61" s="28"/>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="1:4" ht="15.5">
+    <row r="62" spans="1:4" ht="15.75">
       <c r="A62" s="9" t="s">
         <v>1</v>
       </c>
@@ -3277,7 +3335,7 @@
       <c r="C62" s="31"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="1:4" ht="62">
+    <row r="63" spans="1:4" ht="60.75">
       <c r="A63" s="11" t="s">
         <v>49</v>
       </c>
@@ -3286,10 +3344,10 @@
       </c>
       <c r="C63" s="28"/>
       <c r="D63" s="42" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.5">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75">
       <c r="A64" s="11" t="s">
         <v>46</v>
       </c>
@@ -3299,7 +3357,7 @@
       <c r="C64" s="28"/>
       <c r="D64" s="11"/>
     </row>
-    <row r="65" spans="1:4" ht="15.5">
+    <row r="65" spans="1:4" ht="15.75">
       <c r="A65" s="9" t="s">
         <v>1</v>
       </c>
@@ -3308,21 +3366,21 @@
       </c>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="1:4" ht="15.5" customHeight="1">
+    <row r="66" spans="1:4" ht="15.6" customHeight="1">
       <c r="D66" s="47" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="108.5" customHeight="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="108.6" customHeight="1">
       <c r="A67" s="11" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D67" s="48"/>
     </row>
-    <row r="68" spans="1:4" ht="31" customHeight="1">
+    <row r="68" spans="1:4" ht="30.95" customHeight="1">
       <c r="A68" s="9" t="s">
         <v>1</v>
       </c>
@@ -3333,19 +3391,19 @@
     </row>
     <row r="69" spans="1:4">
       <c r="D69" s="47" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="311.5">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="383.25">
       <c r="A70" s="44" t="s">
-        <v>182</v>
+        <v>213</v>
       </c>
       <c r="B70" s="44" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
       <c r="D70" s="48"/>
     </row>
-    <row r="71" spans="1:4" ht="15.5">
+    <row r="71" spans="1:4" ht="15.75">
       <c r="A71" s="9" t="s">
         <v>1</v>
       </c>
@@ -3356,19 +3414,19 @@
     </row>
     <row r="72" spans="1:4">
       <c r="D72" s="47" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="91.5">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="113.25">
       <c r="A73" s="44" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B73" s="44" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D73" s="48"/>
     </row>
-    <row r="74" spans="1:4" ht="15.5">
+    <row r="74" spans="1:4" ht="15.75">
       <c r="A74" s="9" t="s">
         <v>1</v>
       </c>
@@ -3379,13 +3437,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="46" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B76" s="46" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D76" s="47" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -3393,7 +3451,7 @@
       <c r="B77" s="45"/>
       <c r="D77" s="48"/>
     </row>
-    <row r="78" spans="1:4" ht="15.5">
+    <row r="78" spans="1:4" ht="15.75">
       <c r="A78" s="9" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Updated Oracle to SQL Comparison.xlsx
git-tfs-id: [https://payerportfolio.visualstudio.com/]$/USHC_AMER_US_ADU_HSP_Ua3/Source/Utilities/Dev;C1622989
</commit_message>
<xml_diff>
--- a/components/Oracle to SQL Comparison.xlsx
+++ b/components/Oracle to SQL Comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UA3\Source\Utilities\Dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sp9\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2480B46B-7201-4D88-9E04-027D13080F41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6D3EAC2-BF96-4B73-8749-64DF9634FD45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{6185548A-CE3F-4A8C-BB72-B234B9DAD96E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{6185548A-CE3F-4A8C-BB72-B234B9DAD96E}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL to Oracle Syntax" sheetId="1" state="hidden" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="214">
   <si>
     <t>Change Databases in SQL Server vs. Oracle</t>
   </si>
@@ -762,9 +762,6 @@
   <si>
     <t>create index [PROVIDER_LICENSE_IX0] 
   on [UA3_SCREENING].[PROVIDER_LICENSE]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  with (sort_in_tempdb = off, drop_existing = off, ignore_dup_key = off, online = on) on [primary]; </t>
   </si>
   <si>
     <t>alter table [UA3_TENANT].[TENANT]
@@ -1571,13 +1568,13 @@
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="52.28515625" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="52.33203125" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="51.28515625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="60.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="52.28515625" style="8"/>
+    <col min="1" max="1" width="51.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="60.88671875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="52.33203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1602,7 +1599,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="47.25">
+    <row r="3" spans="1:4" ht="46.8">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -1614,7 +1611,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="31.5">
+    <row r="4" spans="1:4" ht="31.2">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -1642,7 +1639,7 @@
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
     </row>
-    <row r="7" spans="1:4" ht="105.75">
+    <row r="7" spans="1:4" ht="105.6">
       <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
@@ -1744,7 +1741,7 @@
       <c r="C16" s="28"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="30.75">
+    <row r="17" spans="1:5" ht="30.6">
       <c r="A17" s="11" t="s">
         <v>19</v>
       </c>
@@ -1806,7 +1803,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30.75">
+    <row r="23" spans="1:5" ht="30.6">
       <c r="A23" s="11" t="s">
         <v>26</v>
       </c>
@@ -1832,7 +1829,7 @@
       <c r="C25" s="31"/>
       <c r="D25" s="35"/>
     </row>
-    <row r="26" spans="1:5" ht="47.25" hidden="1">
+    <row r="26" spans="1:5" ht="46.8" hidden="1">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1863,7 +1860,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="78.75">
+    <row r="28" spans="1:5" ht="78">
       <c r="A28" s="1" t="s">
         <v>113</v>
       </c>
@@ -2053,7 +2050,7 @@
       <c r="C46" s="28"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" ht="31.5">
+    <row r="47" spans="1:4" ht="31.2">
       <c r="A47" s="15" t="s">
         <v>137</v>
       </c>
@@ -2129,7 +2126,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="63">
+    <row r="55" spans="1:4" ht="62.4">
       <c r="A55" s="16" t="s">
         <v>47</v>
       </c>
@@ -2139,7 +2136,7 @@
       <c r="C55" s="28"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" ht="31.5">
+    <row r="56" spans="1:4" ht="31.2">
       <c r="A56" s="5" t="s">
         <v>48</v>
       </c>
@@ -2157,7 +2154,7 @@
       <c r="C57" s="31"/>
       <c r="D57" s="35"/>
     </row>
-    <row r="58" spans="1:4" ht="45.75">
+    <row r="58" spans="1:4" ht="45.6">
       <c r="A58" s="11" t="s">
         <v>49</v>
       </c>
@@ -2197,7 +2194,7 @@
       <c r="C61" s="31"/>
       <c r="D61" s="35"/>
     </row>
-    <row r="62" spans="1:4" ht="45.75">
+    <row r="62" spans="1:4" ht="45.6">
       <c r="A62" s="11" t="s">
         <v>53</v>
       </c>
@@ -2207,7 +2204,7 @@
       <c r="C62" s="28"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4" ht="45.75">
+    <row r="63" spans="1:4" ht="45.6">
       <c r="B63" s="11" t="s">
         <v>121</v>
       </c>
@@ -2307,7 +2304,7 @@
       <c r="C73" s="32"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4" ht="47.25">
+    <row r="74" spans="1:4" ht="46.8">
       <c r="A74" s="19" t="s">
         <v>70</v>
       </c>
@@ -2331,7 +2328,7 @@
       <c r="C76" s="32"/>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4" ht="46.5">
+    <row r="77" spans="1:4" ht="46.2">
       <c r="A77" s="2"/>
       <c r="B77" s="20" t="s">
         <v>122</v>
@@ -2383,7 +2380,7 @@
       <c r="C82" s="32"/>
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="1:4" ht="31.5">
+    <row r="83" spans="1:4" ht="31.2">
       <c r="A83" s="21" t="s">
         <v>78</v>
       </c>
@@ -2401,7 +2398,7 @@
       <c r="C84" s="33"/>
       <c r="D84" s="35"/>
     </row>
-    <row r="85" spans="1:4" ht="30.75">
+    <row r="85" spans="1:4" ht="30.6">
       <c r="A85" s="18" t="s">
         <v>79</v>
       </c>
@@ -2427,7 +2424,7 @@
       <c r="C87" s="32"/>
       <c r="D87" s="3"/>
     </row>
-    <row r="88" spans="1:4" ht="31.5">
+    <row r="88" spans="1:4" ht="31.2">
       <c r="A88" s="19" t="s">
         <v>82</v>
       </c>
@@ -2489,7 +2486,7 @@
       <c r="C94" s="32"/>
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:4" ht="31.5">
+    <row r="95" spans="1:4" ht="31.2">
       <c r="A95" s="21" t="s">
         <v>88</v>
       </c>
@@ -2563,7 +2560,7 @@
       <c r="C102" s="32"/>
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="1:4" ht="31.5">
+    <row r="103" spans="1:4" ht="31.2">
       <c r="A103" s="21" t="s">
         <v>95</v>
       </c>
@@ -2625,7 +2622,7 @@
       <c r="C109" s="33"/>
       <c r="D109" s="35"/>
     </row>
-    <row r="110" spans="1:4" ht="30.75">
+    <row r="110" spans="1:4" ht="30.6">
       <c r="A110" s="18" t="s">
         <v>99</v>
       </c>
@@ -2706,25 +2703,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31552E27-7043-4734-AF5E-4A430D897916}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69:D70"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="49.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="49.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.88671875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75">
+    <row r="1" spans="1:4" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="28"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="15.6">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -2736,7 +2733,7 @@
       </c>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.6">
       <c r="A3" s="11" t="s">
         <v>192</v>
       </c>
@@ -2748,7 +2745,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="15.6">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
@@ -2760,7 +2757,7 @@
       </c>
       <c r="D4" s="50"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="15.6">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
@@ -2770,7 +2767,7 @@
       <c r="C5" s="28"/>
       <c r="D5" s="50"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75">
+    <row r="6" spans="1:4" ht="15.6">
       <c r="A6" s="11" t="s">
         <v>193</v>
       </c>
@@ -2780,7 +2777,7 @@
       <c r="C6" s="28"/>
       <c r="D6" s="50"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75">
+    <row r="7" spans="1:4" ht="15.6">
       <c r="A7" s="11" t="s">
         <v>194</v>
       </c>
@@ -2790,7 +2787,7 @@
       <c r="C7" s="28"/>
       <c r="D7" s="50"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75">
+    <row r="8" spans="1:4" ht="15.6">
       <c r="A8" s="11" t="s">
         <v>195</v>
       </c>
@@ -2800,7 +2797,7 @@
       <c r="C8" s="28"/>
       <c r="D8" s="50"/>
     </row>
-    <row r="9" spans="1:4" ht="30.75">
+    <row r="9" spans="1:4" ht="15.6">
       <c r="A9" s="11" t="s">
         <v>196</v>
       </c>
@@ -2810,7 +2807,7 @@
       <c r="C9" s="28"/>
       <c r="D9" s="50"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75">
+    <row r="10" spans="1:4" ht="15.6">
       <c r="A10" s="11" t="s">
         <v>197</v>
       </c>
@@ -2820,7 +2817,7 @@
       <c r="C10" s="28"/>
       <c r="D10" s="50"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75">
+    <row r="11" spans="1:4" ht="15.6">
       <c r="A11" s="11" t="s">
         <v>198</v>
       </c>
@@ -2830,7 +2827,7 @@
       <c r="C11" s="28"/>
       <c r="D11" s="50"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75">
+    <row r="12" spans="1:4" ht="15.6">
       <c r="A12" s="11" t="s">
         <v>199</v>
       </c>
@@ -2840,7 +2837,7 @@
       <c r="C12" s="28"/>
       <c r="D12" s="50"/>
     </row>
-    <row r="13" spans="1:4" ht="15.75">
+    <row r="13" spans="1:4" ht="15.6">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -2850,7 +2847,7 @@
       <c r="C13" s="28"/>
       <c r="D13" s="50"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75">
+    <row r="14" spans="1:4" ht="15.6">
       <c r="A14" s="1" t="s">
         <v>200</v>
       </c>
@@ -2860,7 +2857,7 @@
       </c>
       <c r="D14" s="50"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75">
+    <row r="15" spans="1:4" ht="15.6">
       <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
@@ -2870,7 +2867,7 @@
       </c>
       <c r="D15" s="50"/>
     </row>
-    <row r="16" spans="1:4" ht="30.75">
+    <row r="16" spans="1:4" ht="30.6">
       <c r="A16" s="11" t="s">
         <v>26</v>
       </c>
@@ -2878,7 +2875,7 @@
       <c r="C16" s="28"/>
       <c r="D16" s="50"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75">
+    <row r="17" spans="1:4" ht="15.6">
       <c r="A17" s="5" t="s">
         <v>150</v>
       </c>
@@ -2886,7 +2883,7 @@
       <c r="C17" s="28"/>
       <c r="D17" s="51"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75">
+    <row r="18" spans="1:4" ht="15.6">
       <c r="A18" s="9" t="s">
         <v>1</v>
       </c>
@@ -2896,7 +2893,7 @@
       <c r="C18" s="31"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" ht="45.75">
+    <row r="19" spans="1:4" ht="45.6">
       <c r="A19" s="11" t="s">
         <v>201</v>
       </c>
@@ -2908,7 +2905,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75">
+    <row r="20" spans="1:4" ht="15.6">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
@@ -2916,7 +2913,7 @@
       <c r="C20" s="28"/>
       <c r="D20" s="53"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75">
+    <row r="21" spans="1:4" ht="15.6">
       <c r="A21" s="11" t="s">
         <v>160</v>
       </c>
@@ -2924,23 +2921,21 @@
       <c r="C21" s="28"/>
       <c r="D21" s="53"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75">
+    <row r="22" spans="1:4" ht="15.6">
       <c r="A22" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="28"/>
       <c r="D22" s="53"/>
     </row>
-    <row r="23" spans="1:4" ht="45.75">
-      <c r="A23" s="11" t="s">
-        <v>202</v>
-      </c>
+    <row r="23" spans="1:4" ht="15.6">
+      <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="28"/>
       <c r="D23" s="53"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75">
+    <row r="24" spans="1:4" ht="15.6">
       <c r="A24" s="11" t="s">
         <v>151</v>
       </c>
@@ -2948,7 +2943,7 @@
       <c r="C24" s="28"/>
       <c r="D24" s="53"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75">
+    <row r="25" spans="1:4" ht="15.6">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -2956,7 +2951,7 @@
       <c r="C25" s="28"/>
       <c r="D25" s="54"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75">
+    <row r="26" spans="1:4" ht="15.6">
       <c r="A26" s="9" t="s">
         <v>1</v>
       </c>
@@ -2966,9 +2961,9 @@
       <c r="C26" s="31"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" ht="47.25">
+    <row r="27" spans="1:4" ht="46.8">
       <c r="A27" s="38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>163</v>
@@ -2980,9 +2975,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="63">
+    <row r="28" spans="1:4" ht="46.8">
       <c r="A28" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B28" s="37" t="s">
         <v>161</v>
@@ -2994,9 +2989,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="63">
+    <row r="29" spans="1:4" ht="46.8">
       <c r="A29" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B29" s="37" t="s">
         <v>112</v>
@@ -3008,9 +3003,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="63">
+    <row r="30" spans="1:4" ht="46.8">
       <c r="A30" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B30" s="37" t="s">
         <v>165</v>
@@ -3022,9 +3017,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="78.75">
+    <row r="31" spans="1:4" ht="78">
       <c r="A31" s="39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>144</v>
@@ -3036,7 +3031,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="63">
+    <row r="32" spans="1:4" ht="62.4">
       <c r="A32" s="1" t="s">
         <v>164</v>
       </c>
@@ -3050,7 +3045,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75">
+    <row r="33" spans="1:4" ht="15.6">
       <c r="A33" s="5" t="s">
         <v>35</v>
       </c>
@@ -3058,7 +3053,7 @@
       <c r="C33" s="28"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75">
+    <row r="34" spans="1:4" ht="15.6">
       <c r="A34" s="9" t="s">
         <v>1</v>
       </c>
@@ -3068,9 +3063,9 @@
       <c r="C34" s="31"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:4" ht="30.75">
+    <row r="35" spans="1:4" ht="15.6">
       <c r="A35" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>37</v>
@@ -3082,7 +3077,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75">
+    <row r="36" spans="1:4" ht="15.6">
       <c r="A36" s="11" t="s">
         <v>38</v>
       </c>
@@ -3092,7 +3087,7 @@
       <c r="C36" s="28"/>
       <c r="D36" s="53"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75">
+    <row r="37" spans="1:4" ht="15.6">
       <c r="A37" s="11" t="s">
         <v>39</v>
       </c>
@@ -3102,7 +3097,7 @@
       <c r="C37" s="28"/>
       <c r="D37" s="53"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75">
+    <row r="38" spans="1:4" ht="15.6">
       <c r="A38" s="11" t="s">
         <v>41</v>
       </c>
@@ -3110,7 +3105,7 @@
       <c r="C38" s="28"/>
       <c r="D38" s="53"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75">
+    <row r="39" spans="1:4" ht="15.6">
       <c r="A39" s="15" t="s">
         <v>6</v>
       </c>
@@ -3118,9 +3113,9 @@
       <c r="C39" s="28"/>
       <c r="D39" s="54"/>
     </row>
-    <row r="40" spans="1:4" ht="47.25">
+    <row r="40" spans="1:4" ht="46.8">
       <c r="A40" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>155</v>
@@ -3132,7 +3127,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75">
+    <row r="41" spans="1:4" ht="15.6">
       <c r="A41" s="15" t="s">
         <v>6</v>
       </c>
@@ -3140,13 +3135,13 @@
       <c r="C41" s="28"/>
       <c r="D41" s="56"/>
     </row>
-    <row r="42" spans="1:4" ht="15.75">
+    <row r="42" spans="1:4" ht="15.6">
       <c r="A42" s="15"/>
       <c r="B42" s="11"/>
       <c r="C42" s="28"/>
       <c r="D42" s="56"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75">
+    <row r="43" spans="1:4" ht="15.6">
       <c r="A43" s="5" t="s">
         <v>42</v>
       </c>
@@ -3154,7 +3149,7 @@
       <c r="C43" s="28"/>
       <c r="D43" s="57"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75">
+    <row r="44" spans="1:4" ht="15.6">
       <c r="A44" s="9" t="s">
         <v>1</v>
       </c>
@@ -3164,9 +3159,9 @@
       <c r="C44" s="31"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:4" ht="30.75">
+    <row r="45" spans="1:4" ht="15.6">
       <c r="A45" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>37</v>
@@ -3178,7 +3173,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75">
+    <row r="46" spans="1:4" ht="15.6">
       <c r="A46" s="11" t="s">
         <v>136</v>
       </c>
@@ -3188,7 +3183,7 @@
       <c r="C46" s="28"/>
       <c r="D46" s="56"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75">
+    <row r="47" spans="1:4" ht="15.6">
       <c r="A47" s="11" t="s">
         <v>139</v>
       </c>
@@ -3198,7 +3193,7 @@
       <c r="C47" s="28"/>
       <c r="D47" s="56"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75">
+    <row r="48" spans="1:4" ht="15.6">
       <c r="A48" s="11" t="s">
         <v>108</v>
       </c>
@@ -3208,7 +3203,7 @@
       <c r="C48" s="28"/>
       <c r="D48" s="56"/>
     </row>
-    <row r="49" spans="1:4" ht="31.5">
+    <row r="49" spans="1:4" ht="31.2">
       <c r="A49" s="15" t="s">
         <v>137</v>
       </c>
@@ -3216,23 +3211,23 @@
       <c r="C49" s="28"/>
       <c r="D49" s="56"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75">
+    <row r="50" spans="1:4" ht="15.6">
       <c r="A50" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="28"/>
       <c r="D50" s="56"/>
     </row>
-    <row r="51" spans="1:4" ht="15.75">
+    <row r="51" spans="1:4" ht="15.6">
       <c r="A51" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="28"/>
       <c r="D51" s="56"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75">
+    <row r="52" spans="1:4" ht="15.6">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -3241,9 +3236,9 @@
       </c>
       <c r="D52" s="57"/>
     </row>
-    <row r="53" spans="1:4" ht="60.75">
+    <row r="53" spans="1:4" ht="60.6">
       <c r="A53" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>156</v>
@@ -3253,7 +3248,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75">
+    <row r="54" spans="1:4" ht="15.6">
       <c r="A54" s="1" t="s">
         <v>6</v>
       </c>
@@ -3261,13 +3256,13 @@
       <c r="C54" s="28"/>
       <c r="D54" s="11"/>
     </row>
-    <row r="55" spans="1:4" ht="15.75">
+    <row r="55" spans="1:4" ht="15.6">
       <c r="A55" s="1"/>
       <c r="B55" s="11"/>
       <c r="C55" s="28"/>
       <c r="D55" s="11"/>
     </row>
-    <row r="56" spans="1:4" ht="31.5">
+    <row r="56" spans="1:4" ht="31.2">
       <c r="A56" s="5" t="s">
         <v>45</v>
       </c>
@@ -3275,7 +3270,7 @@
       <c r="C56" s="28"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="1:4" ht="15.75">
+    <row r="57" spans="1:4" ht="15.6">
       <c r="A57" s="9" t="s">
         <v>1</v>
       </c>
@@ -3285,19 +3280,19 @@
       <c r="C57" s="31"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="1:4" ht="180.75">
+    <row r="58" spans="1:4" ht="180.6">
       <c r="A58" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B58" s="11" t="s">
         <v>211</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>212</v>
       </c>
       <c r="C58" s="28"/>
       <c r="D58" s="43" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75">
+    <row r="59" spans="1:4" ht="15.6">
       <c r="A59" s="11" t="s">
         <v>46</v>
       </c>
@@ -3305,7 +3300,7 @@
       <c r="C59" s="28"/>
       <c r="D59" s="11"/>
     </row>
-    <row r="60" spans="1:4" ht="63">
+    <row r="60" spans="1:4" ht="62.4">
       <c r="A60" s="16" t="s">
         <v>47</v>
       </c>
@@ -3317,7 +3312,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="31.5">
+    <row r="61" spans="1:4" ht="31.2">
       <c r="A61" s="5" t="s">
         <v>48</v>
       </c>
@@ -3325,7 +3320,7 @@
       <c r="C61" s="28"/>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="1:4" ht="15.75">
+    <row r="62" spans="1:4" ht="15.6">
       <c r="A62" s="9" t="s">
         <v>1</v>
       </c>
@@ -3335,7 +3330,7 @@
       <c r="C62" s="31"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="1:4" ht="60.75">
+    <row r="63" spans="1:4" ht="60.6">
       <c r="A63" s="11" t="s">
         <v>49</v>
       </c>
@@ -3347,7 +3342,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.75">
+    <row r="64" spans="1:4" ht="15.6">
       <c r="A64" s="11" t="s">
         <v>46</v>
       </c>
@@ -3357,7 +3352,7 @@
       <c r="C64" s="28"/>
       <c r="D64" s="11"/>
     </row>
-    <row r="65" spans="1:4" ht="15.75">
+    <row r="65" spans="1:4" ht="15.6">
       <c r="A65" s="9" t="s">
         <v>1</v>
       </c>
@@ -3380,7 +3375,7 @@
       </c>
       <c r="D67" s="48"/>
     </row>
-    <row r="68" spans="1:4" ht="30.95" customHeight="1">
+    <row r="68" spans="1:4" ht="30.9" customHeight="1">
       <c r="A68" s="9" t="s">
         <v>1</v>
       </c>
@@ -3394,16 +3389,16 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="383.25">
+    <row r="70" spans="1:4" ht="317.39999999999998">
       <c r="A70" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="B70" s="44" t="s">
-        <v>214</v>
-      </c>
       <c r="D70" s="48"/>
     </row>
-    <row r="71" spans="1:4" ht="15.75">
+    <row r="71" spans="1:4" ht="15.6">
       <c r="A71" s="9" t="s">
         <v>1</v>
       </c>
@@ -3417,7 +3412,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="113.25">
+    <row r="73" spans="1:4" ht="93">
       <c r="A73" s="44" t="s">
         <v>176</v>
       </c>
@@ -3426,7 +3421,7 @@
       </c>
       <c r="D73" s="48"/>
     </row>
-    <row r="74" spans="1:4" ht="15.75">
+    <row r="74" spans="1:4" ht="15.6">
       <c r="A74" s="9" t="s">
         <v>1</v>
       </c>
@@ -3451,7 +3446,7 @@
       <c r="B77" s="45"/>
       <c r="D77" s="48"/>
     </row>
-    <row r="78" spans="1:4" ht="15.75">
+    <row r="78" spans="1:4" ht="15.6">
       <c r="A78" s="9" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Update to qualify tables in Oracle
git-tfs-id: [https://payerportfolio.visualstudio.com/]$/USHC_AMER_US_ADU_HSP_Ua3/Source/Utilities/Dev;C1627144
</commit_message>
<xml_diff>
--- a/components/Oracle to SQL Comparison.xlsx
+++ b/components/Oracle to SQL Comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sp9\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UA3\USHC_AMER_US_ADU_HSP_Ua3\Source\Utilities\Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6D3EAC2-BF96-4B73-8749-64DF9634FD45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC34E92-DA68-428C-A161-60F42EFC3416}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{6185548A-CE3F-4A8C-BB72-B234B9DAD96E}"/>
+    <workbookView xWindow="31305" yWindow="1335" windowWidth="18180" windowHeight="10800" firstSheet="1" activeTab="1" xr2:uid="{6185548A-CE3F-4A8C-BB72-B234B9DAD96E}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL to Oracle Syntax" sheetId="1" state="hidden" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="221">
   <si>
     <t>Change Databases in SQL Server vs. Oracle</t>
   </si>
@@ -589,56 +589,26 @@
     <t xml:space="preserve">GO </t>
   </si>
   <si>
-    <t>alter table POTENTIAL_TPL_CLAIM 
-  rename to PAID_CLAIM;</t>
-  </si>
-  <si>
     <t>Add PK Constraint</t>
   </si>
   <si>
     <t>Add FK Constraint</t>
   </si>
   <si>
-    <t>alter table PAID_CLAIM 
-  rename constraint POTENTIAL_TPL_CLAIM_PK 
-    to PAID_CLAIM_PK;</t>
-  </si>
-  <si>
-    <t>alter table PAID_CLAIM 
-  rename constraint POTENTIAL_TPL_CLAIM_FK0 
-    to PAID_CLAIM_FK0;</t>
-  </si>
-  <si>
     <t>Rename FK Constraint</t>
   </si>
   <si>
     <t>Mention Data Compression</t>
   </si>
   <si>
-    <t xml:space="preserve">create index PROVIDER_LICENSE_IX0 
-  on PROVIDER_LICENSE(LICENSE_NUMBER_TXT); </t>
-  </si>
-  <si>
     <t>(LICENSE_NUMBER_TXT)</t>
   </si>
   <si>
-    <t>ALTER TABLE TENANT 
-MODIFY (TENANT_NAME varchar(200) NOT NULL);</t>
-  </si>
-  <si>
     <t>Modify null\not null constraint</t>
-  </si>
-  <si>
-    <t>ALTER TABLE TENANT
-ADD TENANT_NAME varchar(150) NULL;</t>
   </si>
   <si>
     <t>EXEC SP_RENAME 'UA3_TPL_POLICY.POTENTIAL_TPL_CLAIM', 'PAID_CLAIM'
 GO</t>
-  </si>
-  <si>
-    <t>ALTER TABLE TENANT 
-MODIFY (TENANT_NAME varchar(200));</t>
   </si>
   <si>
     <t>Modify column - specify NULL / NOT null</t>
@@ -844,6 +814,59 @@
 update UA3_INTEGRATION.MODULE_EVENTS set EVENT_TYPE_NAME = 'ExpenditureRequestUpdated', MODIFIED_TS = sys_extract_utc(systimestamp) 
 where EVENT_TYPE_NAME = 'HIPPExpenditureRequestUpdated'; 
 commit;</t>
+  </si>
+  <si>
+    <t>UA3_TENANT.APPLICATION</t>
+  </si>
+  <si>
+    <t>LICENSE_NUMBER_TXT</t>
+  </si>
+  <si>
+    <t>create index PROVIDER_LICENSE_IX0 
+  on UA3_SCREENING.PROVIDER_LICENSE</t>
+  </si>
+  <si>
+    <t>ALTER UA3_TENANT.TABLE TENANT
+ADD TENANT_NAME varchar(150) NULL;</t>
+  </si>
+  <si>
+    <t>ALTER UA3_TENANT.TABLE TENANT 
+MODIFY (TENANT_NAME varchar(200) NOT NULL);</t>
+  </si>
+  <si>
+    <t>ALTER UA3_TENANT.TABLE TENANT 
+MODIFY (TENANT_NAME NOT NULL);</t>
+  </si>
+  <si>
+    <t>ALTER UA3_TENANT.TABLE TENANT 
+MODIFY (TENANT_NAME varchar(200));</t>
+  </si>
+  <si>
+    <t>ALTER TABLE UA3_INTEGRATION.ETF_OUTBOUND_METADATA_DEFN 
+RENAME COLUMN ETF_OUTBOUND_EXTRACT_ID to ETF_OUTBOUND_EXTRACT_NAME;</t>
+  </si>
+  <si>
+    <t>alter table UA3_TPL_POLICY.POTENTIAL_TPL_CLAIM 
+  rename to PAID_CLAIM;</t>
+  </si>
+  <si>
+    <t>ALTER TABLE UA3_TENANT.APPLICATION</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT APPLICATION_PK</t>
+  </si>
+  <si>
+    <t>alter table UA3_TPL_POLICY.PAID_CLAIM 
+  rename constraint POTENTIAL_TPL_CLAIM_PK 
+    to PAID_CLAIM_PK;</t>
+  </si>
+  <si>
+    <t>REFERENCES UA3_TENANT.MODULE (MODULE_ID);</t>
+  </si>
+  <si>
+    <t>alter table UA3_TPL_POLICY.PAID_CLAIM 
+  rename constraint POTENTIAL_TPL_CLAIM_FK0 
+    to PAID_CLAIM_FK0;</t>
   </si>
 </sst>
 </file>
@@ -2703,8 +2726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31552E27-7043-4734-AF5E-4A430D897916}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49.109375" defaultRowHeight="14.4"/>
@@ -2735,14 +2758,14 @@
     </row>
     <row r="3" spans="1:4" ht="15.6">
       <c r="A3" s="11" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="49" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.6">
@@ -2750,7 +2773,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>207</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>14</v>
@@ -2769,7 +2792,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.6">
       <c r="A6" s="11" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>128</v>
@@ -2779,7 +2802,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.6">
       <c r="A7" s="11" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>129</v>
@@ -2789,7 +2812,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.6">
       <c r="A8" s="11" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>130</v>
@@ -2799,7 +2822,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.6">
       <c r="A9" s="11" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>131</v>
@@ -2809,7 +2832,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.6">
       <c r="A10" s="11" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>132</v>
@@ -2819,7 +2842,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.6">
       <c r="A11" s="11" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>133</v>
@@ -2829,7 +2852,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.6">
       <c r="A12" s="11" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>134</v>
@@ -2849,11 +2872,11 @@
     </row>
     <row r="14" spans="1:4" ht="15.6">
       <c r="A14" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="28" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D14" s="50"/>
     </row>
@@ -2895,29 +2918,33 @@
     </row>
     <row r="19" spans="1:4" ht="45.6">
       <c r="A19" s="11" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>159</v>
+        <v>209</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="52" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.6">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="C20" s="28"/>
       <c r="D20" s="53"/>
     </row>
     <row r="21" spans="1:4" ht="15.6">
       <c r="A21" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="B21" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="C21" s="28"/>
       <c r="D21" s="53"/>
     </row>
@@ -2925,7 +2952,9 @@
       <c r="A22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="C22" s="28"/>
       <c r="D22" s="53"/>
     </row>
@@ -2963,86 +2992,86 @@
     </row>
     <row r="27" spans="1:4" ht="46.8">
       <c r="A27" s="38" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>163</v>
+        <v>210</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="46.8">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="62.4">
       <c r="A28" s="3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>161</v>
+        <v>211</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="46.8">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="62.4">
       <c r="A29" s="3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>112</v>
+        <v>212</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="46.8">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="62.4">
       <c r="A30" s="3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>165</v>
+        <v>213</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="78">
       <c r="A31" s="39" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>144</v>
+        <v>214</v>
       </c>
       <c r="C31" s="28" t="s">
         <v>145</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="62.4">
       <c r="A32" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>152</v>
+        <v>215</v>
       </c>
       <c r="C32" s="28" t="s">
         <v>147</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.6">
@@ -3065,24 +3094,24 @@
     </row>
     <row r="35" spans="1:4" ht="15.6">
       <c r="A35" s="11" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>216</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.6">
       <c r="A36" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>38</v>
+      <c r="B36" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="C36" s="28"/>
       <c r="D36" s="53"/>
@@ -3091,7 +3120,7 @@
       <c r="A37" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C37" s="28"/>
@@ -3115,16 +3144,16 @@
     </row>
     <row r="40" spans="1:4" ht="46.8">
       <c r="A40" s="15" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>155</v>
+        <v>218</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>149</v>
       </c>
       <c r="D40" s="55" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.6">
@@ -3161,16 +3190,16 @@
     </row>
     <row r="45" spans="1:4" ht="15.6">
       <c r="A45" s="11" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>37</v>
+        <v>216</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D45" s="55" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.6">
@@ -3193,12 +3222,12 @@
       <c r="C47" s="28"/>
       <c r="D47" s="56"/>
     </row>
-    <row r="48" spans="1:4" ht="15.6">
+    <row r="48" spans="1:4" ht="30.6">
       <c r="A48" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>110</v>
+        <v>219</v>
       </c>
       <c r="C48" s="28"/>
       <c r="D48" s="56"/>
@@ -3213,7 +3242,7 @@
     </row>
     <row r="50" spans="1:4" ht="15.6">
       <c r="A50" s="15" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="28"/>
@@ -3221,7 +3250,7 @@
     </row>
     <row r="51" spans="1:4" ht="15.6">
       <c r="A51" s="15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="28"/>
@@ -3232,20 +3261,20 @@
         <v>6</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D52" s="57"/>
     </row>
     <row r="53" spans="1:4" ht="60.6">
       <c r="A53" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>156</v>
+        <v>220</v>
       </c>
       <c r="C53" s="28"/>
       <c r="D53" s="42" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.6">
@@ -3282,14 +3311,14 @@
     </row>
     <row r="58" spans="1:4" ht="180.6">
       <c r="A58" s="11" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C58" s="28"/>
       <c r="D58" s="43" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.6">
@@ -3309,7 +3338,7 @@
       </c>
       <c r="C60" s="28"/>
       <c r="D60" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="31.2">
@@ -3339,7 +3368,7 @@
       </c>
       <c r="C63" s="28"/>
       <c r="D63" s="42" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.6">
@@ -3363,15 +3392,15 @@
     </row>
     <row r="66" spans="1:4" ht="15.6" customHeight="1">
       <c r="D66" s="47" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="108.6" customHeight="1">
       <c r="A67" s="11" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D67" s="48"/>
     </row>
@@ -3386,15 +3415,15 @@
     </row>
     <row r="69" spans="1:4">
       <c r="D69" s="47" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="317.39999999999998">
       <c r="A70" s="44" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B70" s="44" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D70" s="48"/>
     </row>
@@ -3409,15 +3438,15 @@
     </row>
     <row r="72" spans="1:4">
       <c r="D72" s="47" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="93">
       <c r="A73" s="44" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B73" s="44" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D73" s="48"/>
     </row>
@@ -3432,13 +3461,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="46" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B76" s="46" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D76" s="47" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" spans="1:4">

</xml_diff>

<commit_message>
Minor update - [objectname] vs (objectname) for SQLServer
git-tfs-id: [https://payerportfolio.visualstudio.com/]$/USHC_AMER_US_ADU_HSP_Ua3/Source/Utilities/Dev;C1632550
</commit_message>
<xml_diff>
--- a/components/Oracle to SQL Comparison.xlsx
+++ b/components/Oracle to SQL Comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/sreedhar_puppala_dxc_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UA3\source\Utilities\Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A4ED669-5E0B-4A0E-B033-244232AE68DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D8CBEA-7E99-4B71-BACB-607C95F3E185}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{6185548A-CE3F-4A8C-BB72-B234B9DAD96E}"/>
   </bookViews>
@@ -601,9 +601,6 @@
     <t>Mention Data Compression</t>
   </si>
   <si>
-    <t>(LICENSE_NUMBER_TXT)</t>
-  </si>
-  <si>
     <t>Modify null\not null constraint</t>
   </si>
   <si>
@@ -896,6 +893,9 @@
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>[LICENSE_NUMBER_TXT]</t>
   </si>
 </sst>
 </file>
@@ -2756,7 +2756,7 @@
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49.109375" defaultRowHeight="14.4"/>
@@ -2787,14 +2787,14 @@
     </row>
     <row r="3" spans="1:4" ht="15.6">
       <c r="A3" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.6">
@@ -2802,7 +2802,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>14</v>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.6">
       <c r="A6" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>128</v>
@@ -2831,7 +2831,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.6">
       <c r="A7" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>129</v>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.6">
       <c r="A8" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>130</v>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.6">
       <c r="A9" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>131</v>
@@ -2861,7 +2861,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.6">
       <c r="A10" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>132</v>
@@ -2871,7 +2871,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.6">
       <c r="A11" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>133</v>
@@ -2881,7 +2881,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.6">
       <c r="A12" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>134</v>
@@ -2901,7 +2901,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.6">
       <c r="A14" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="28" t="s">
@@ -2947,28 +2947,28 @@
     </row>
     <row r="19" spans="1:4" ht="225.6">
       <c r="A19" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C19" s="28" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45.6">
       <c r="A20" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.6">
@@ -2983,10 +2983,10 @@
     </row>
     <row r="22" spans="1:4" ht="15.6">
       <c r="A22" s="11" t="s">
-        <v>156</v>
+        <v>226</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="53"/>
@@ -2996,17 +2996,17 @@
         <v>24</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="53"/>
     </row>
     <row r="24" spans="1:4" ht="15.6">
       <c r="A24" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C24" s="28"/>
       <c r="D24" s="53"/>
@@ -3016,7 +3016,7 @@
         <v>151</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="53"/>
@@ -3041,86 +3041,86 @@
     </row>
     <row r="28" spans="1:4" ht="46.8">
       <c r="A28" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>30</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="46.8">
       <c r="A29" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="46.8">
       <c r="A30" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="46.8">
       <c r="A31" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D31" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="78">
       <c r="A32" s="39" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C32" s="28" t="s">
         <v>145</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="62.4">
       <c r="A33" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>147</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.6">
@@ -3143,16 +3143,16 @@
     </row>
     <row r="36" spans="1:4" ht="15.6">
       <c r="A36" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>152</v>
       </c>
       <c r="D36" s="52" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.6">
@@ -3160,7 +3160,7 @@
         <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C37" s="28"/>
       <c r="D37" s="53"/>
@@ -3193,16 +3193,16 @@
     </row>
     <row r="41" spans="1:4" ht="46.8">
       <c r="A41" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C41" s="28" t="s">
         <v>149</v>
       </c>
       <c r="D41" s="55" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.6">
@@ -3239,16 +3239,16 @@
     </row>
     <row r="46" spans="1:4" ht="15.6">
       <c r="A46" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C46" s="28" t="s">
         <v>153</v>
       </c>
       <c r="D46" s="55" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.6">
@@ -3276,7 +3276,7 @@
         <v>108</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C49" s="28"/>
       <c r="D49" s="56"/>
@@ -3291,7 +3291,7 @@
     </row>
     <row r="51" spans="1:4" ht="15.6">
       <c r="A51" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="28"/>
@@ -3299,7 +3299,7 @@
     </row>
     <row r="52" spans="1:4" ht="15.6">
       <c r="A52" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B52" s="15"/>
       <c r="C52" s="28"/>
@@ -3316,14 +3316,14 @@
     </row>
     <row r="54" spans="1:4" ht="60.6">
       <c r="A54" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C54" s="28"/>
       <c r="D54" s="42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.6">
@@ -3360,14 +3360,14 @@
     </row>
     <row r="59" spans="1:4" ht="180.6">
       <c r="A59" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B59" s="11" t="s">
         <v>203</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>204</v>
       </c>
       <c r="C59" s="28"/>
       <c r="D59" s="43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.6">
@@ -3387,7 +3387,7 @@
       </c>
       <c r="C61" s="28"/>
       <c r="D61" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="31.2">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="C64" s="28"/>
       <c r="D64" s="42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.6">
@@ -3441,15 +3441,15 @@
     </row>
     <row r="67" spans="1:4" ht="15.6" customHeight="1">
       <c r="D67" s="47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="108.6" customHeight="1">
       <c r="A68" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D68" s="48"/>
     </row>
@@ -3464,15 +3464,15 @@
     </row>
     <row r="70" spans="1:4">
       <c r="D70" s="47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="317.39999999999998">
       <c r="A71" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="B71" s="44" t="s">
         <v>205</v>
-      </c>
-      <c r="B71" s="44" t="s">
-        <v>206</v>
       </c>
       <c r="D71" s="48"/>
     </row>
@@ -3487,15 +3487,15 @@
     </row>
     <row r="73" spans="1:4">
       <c r="D73" s="47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="93">
       <c r="A74" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="B74" s="44" t="s">
         <v>169</v>
-      </c>
-      <c r="B74" s="44" t="s">
-        <v>170</v>
       </c>
       <c r="D74" s="48"/>
     </row>
@@ -3510,13 +3510,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="B77" s="46" t="s">
+      <c r="D77" s="47" t="s">
         <v>174</v>
-      </c>
-      <c r="D77" s="47" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:4">

</xml_diff>